<commit_message>
Main loon refactored Safe mode added To do: 	Error logs
</commit_message>
<xml_diff>
--- a/2_2024.xlsx
+++ b/2_2024.xlsx
@@ -17,10 +17,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot;zł&quot;"/>
     <numFmt numFmtId="166" formatCode="dd\ mmm"/>
+    <numFmt numFmtId="167" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -60,7 +61,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -83,18 +84,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD966"/>
         <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FF9933"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,18 +181,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -228,6 +205,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
@@ -286,18 +275,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -320,6 +297,18 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -686,7 +675,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -982,7 +971,7 @@
       <c r="H5" s="33" t="n"/>
       <c r="I5" s="33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>N</t>
         </is>
       </c>
       <c r="L5" s="46" t="n">
@@ -1040,7 +1029,7 @@
       <c r="H6" s="36" t="n"/>
       <c r="I6" s="36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>N</t>
         </is>
       </c>
       <c r="L6" s="40" t="n">
@@ -1072,33 +1061,33 @@
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="32">
-      <c r="A7" s="52" t="inlineStr">
+      <c r="A7" s="42" t="inlineStr">
         <is>
           <t>p1</t>
         </is>
       </c>
-      <c r="B7" s="52" t="inlineStr">
+      <c r="B7" s="42" t="inlineStr">
         <is>
           <t>pawel1</t>
         </is>
       </c>
-      <c r="C7" s="52" t="n">
+      <c r="C7" s="42" t="n">
         <v>10</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="43">
         <f>SUM(R2:R30)</f>
         <v/>
       </c>
-      <c r="E7" s="54" t="n"/>
-      <c r="F7" s="54" t="n"/>
-      <c r="G7" s="55">
+      <c r="E7" s="44" t="n"/>
+      <c r="F7" s="44" t="n"/>
+      <c r="G7" s="45">
         <f>((D7*24)*C7)-E7-F7</f>
         <v/>
       </c>
-      <c r="H7" s="52" t="n"/>
-      <c r="I7" s="52" t="inlineStr">
-        <is>
-          <t>T</t>
+      <c r="H7" s="42" t="n"/>
+      <c r="I7" s="42" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
       <c r="L7" s="46" t="n">
@@ -1130,7 +1119,7 @@
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="32">
-      <c r="B8" s="56" t="n"/>
+      <c r="B8" s="52" t="n"/>
       <c r="L8" s="40" t="n">
         <v>45329</v>
       </c>
@@ -1813,19 +1802,19 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="32">
-      <c r="A1" s="57" t="n"/>
+      <c r="A1" s="53" t="n"/>
       <c r="B1" s="33" t="inlineStr">
         <is>
           <t>marcin0</t>
         </is>
       </c>
-      <c r="C1" s="57" t="inlineStr">
+      <c r="C1" s="53" t="inlineStr">
         <is>
           <t>t1</t>
         </is>
@@ -1835,7 +1824,7 @@
           <t>marcin1</t>
         </is>
       </c>
-      <c r="E1" s="57" t="inlineStr">
+      <c r="E1" s="53" t="inlineStr">
         <is>
           <t>t2</t>
         </is>
@@ -1845,7 +1834,7 @@
           <t>marcin2</t>
         </is>
       </c>
-      <c r="G1" s="57" t="inlineStr">
+      <c r="G1" s="53" t="inlineStr">
         <is>
           <t>t3</t>
         </is>
@@ -1855,7 +1844,7 @@
           <t>marcin3</t>
         </is>
       </c>
-      <c r="I1" s="57" t="inlineStr">
+      <c r="I1" s="53" t="inlineStr">
         <is>
           <t>t4</t>
         </is>
@@ -1865,7 +1854,7 @@
           <t>marcin5</t>
         </is>
       </c>
-      <c r="K1" s="57" t="inlineStr">
+      <c r="K1" s="53" t="inlineStr">
         <is>
           <t>t5</t>
         </is>
@@ -1875,504 +1864,516 @@
           <t>pawel1</t>
         </is>
       </c>
-      <c r="M1" s="57" t="inlineStr">
+      <c r="M1" s="53" t="inlineStr">
         <is>
           <t>p1</t>
         </is>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="32">
-      <c r="A2" s="58" t="n">
+      <c r="A2" s="54" t="n">
         <v>45323</v>
       </c>
       <c r="B2" s="36" t="n"/>
-      <c r="C2" s="59" t="n"/>
+      <c r="C2" s="55" t="n"/>
       <c r="D2" s="36" t="n"/>
-      <c r="E2" s="59" t="n"/>
+      <c r="E2" s="55" t="n"/>
       <c r="F2" s="36" t="n"/>
-      <c r="G2" s="59" t="n"/>
+      <c r="G2" s="55" t="n"/>
       <c r="H2" s="36" t="n"/>
-      <c r="I2" s="59" t="n"/>
+      <c r="I2" s="55" t="n"/>
       <c r="J2" s="36" t="n"/>
-      <c r="K2" s="59" t="n"/>
+      <c r="K2" s="55" t="n"/>
       <c r="L2" s="36" t="n"/>
-      <c r="M2" s="59" t="n"/>
+      <c r="M2" s="55" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="32">
-      <c r="A3" s="60" t="n">
+      <c r="A3" s="56" t="n">
         <v>45324</v>
       </c>
       <c r="B3" s="33" t="n"/>
-      <c r="C3" s="57" t="n"/>
+      <c r="C3" s="53" t="n"/>
       <c r="D3" s="33" t="n"/>
-      <c r="E3" s="57" t="n"/>
+      <c r="E3" s="53" t="n"/>
       <c r="F3" s="33" t="n"/>
-      <c r="G3" s="57" t="n"/>
+      <c r="G3" s="53" t="n"/>
       <c r="H3" s="33" t="n"/>
-      <c r="I3" s="57" t="n"/>
+      <c r="I3" s="53" t="n"/>
       <c r="J3" s="33" t="n"/>
-      <c r="K3" s="57" t="n"/>
+      <c r="K3" s="53" t="n"/>
       <c r="L3" s="33" t="n"/>
-      <c r="M3" s="57" t="n"/>
+      <c r="M3" s="53" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1" s="32">
-      <c r="A4" s="61" t="n">
+      <c r="A4" s="57" t="n">
         <v>45325</v>
       </c>
-      <c r="B4" s="62" t="n"/>
-      <c r="C4" s="63" t="n"/>
-      <c r="D4" s="62" t="n"/>
-      <c r="E4" s="63" t="n"/>
-      <c r="F4" s="62" t="n"/>
-      <c r="G4" s="63" t="n"/>
-      <c r="H4" s="62" t="n"/>
-      <c r="I4" s="63" t="n"/>
-      <c r="J4" s="62" t="n"/>
-      <c r="K4" s="63" t="n"/>
-      <c r="L4" s="62" t="n"/>
-      <c r="M4" s="63" t="n"/>
+      <c r="B4" s="58" t="n"/>
+      <c r="C4" s="59" t="n"/>
+      <c r="D4" s="58" t="n"/>
+      <c r="E4" s="59" t="n"/>
+      <c r="F4" s="58" t="n"/>
+      <c r="G4" s="59" t="n"/>
+      <c r="H4" s="58" t="n"/>
+      <c r="I4" s="59" t="n"/>
+      <c r="J4" s="58" t="n"/>
+      <c r="K4" s="59" t="n"/>
+      <c r="L4" s="58" t="n"/>
+      <c r="M4" s="59" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1" s="32">
-      <c r="A5" s="61" t="n">
+      <c r="A5" s="57" t="n">
         <v>45326</v>
       </c>
-      <c r="B5" s="62" t="n"/>
-      <c r="C5" s="63" t="n"/>
-      <c r="D5" s="62" t="n"/>
-      <c r="E5" s="63" t="n"/>
-      <c r="F5" s="62" t="n"/>
-      <c r="G5" s="63" t="n"/>
-      <c r="H5" s="62" t="n"/>
-      <c r="I5" s="63" t="n"/>
-      <c r="J5" s="62" t="n"/>
-      <c r="K5" s="63" t="n"/>
-      <c r="L5" s="62" t="n"/>
-      <c r="M5" s="63" t="n"/>
+      <c r="B5" s="58" t="n"/>
+      <c r="C5" s="59" t="n"/>
+      <c r="D5" s="58" t="n"/>
+      <c r="E5" s="59" t="n"/>
+      <c r="F5" s="58" t="n"/>
+      <c r="G5" s="59" t="n"/>
+      <c r="H5" s="58" t="n"/>
+      <c r="I5" s="59" t="n"/>
+      <c r="J5" s="58" t="n"/>
+      <c r="K5" s="59" t="n"/>
+      <c r="L5" s="58" t="n"/>
+      <c r="M5" s="59" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1" s="32">
-      <c r="A6" s="58" t="n">
+      <c r="A6" s="54" t="n">
         <v>45327</v>
       </c>
       <c r="B6" s="36" t="n"/>
-      <c r="C6" s="59" t="n"/>
+      <c r="C6" s="55" t="n"/>
       <c r="D6" s="36" t="n"/>
-      <c r="E6" s="59" t="n"/>
+      <c r="E6" s="55" t="n"/>
       <c r="F6" s="36" t="n"/>
-      <c r="G6" s="59" t="n"/>
+      <c r="G6" s="55" t="n"/>
       <c r="H6" s="36" t="n"/>
-      <c r="I6" s="59" t="n"/>
+      <c r="I6" s="55" t="n"/>
       <c r="J6" s="36" t="n"/>
-      <c r="K6" s="59" t="n"/>
+      <c r="K6" s="55" t="n"/>
       <c r="L6" s="36" t="n"/>
-      <c r="M6" s="59" t="n"/>
+      <c r="M6" s="55" t="n"/>
     </row>
     <row r="7" ht="15" customHeight="1" s="32">
-      <c r="A7" s="60" t="n">
+      <c r="A7" s="56" t="n">
         <v>45328</v>
       </c>
       <c r="B7" s="33" t="n"/>
-      <c r="C7" s="57" t="n"/>
+      <c r="C7" s="53" t="n"/>
       <c r="D7" s="33" t="n"/>
-      <c r="E7" s="57" t="n"/>
+      <c r="E7" s="53" t="n"/>
       <c r="F7" s="33" t="n"/>
-      <c r="G7" s="57" t="n"/>
+      <c r="G7" s="53" t="n"/>
       <c r="H7" s="33" t="n"/>
-      <c r="I7" s="57" t="n"/>
+      <c r="I7" s="53" t="n"/>
       <c r="J7" s="33" t="n"/>
-      <c r="K7" s="57" t="n"/>
+      <c r="K7" s="53" t="n"/>
       <c r="L7" s="33" t="n"/>
-      <c r="M7" s="57" t="n"/>
+      <c r="M7" s="53" t="n"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="32">
-      <c r="A8" s="58" t="n">
+      <c r="A8" s="54" t="n">
         <v>45329</v>
       </c>
       <c r="B8" s="36" t="n"/>
-      <c r="C8" s="59" t="n"/>
+      <c r="C8" s="55" t="n"/>
       <c r="D8" s="36" t="n"/>
-      <c r="E8" s="59" t="n"/>
+      <c r="E8" s="55" t="n"/>
       <c r="F8" s="36" t="n"/>
-      <c r="G8" s="59" t="n"/>
+      <c r="G8" s="55" t="n"/>
       <c r="H8" s="36" t="n"/>
-      <c r="I8" s="59" t="n"/>
+      <c r="I8" s="55" t="n"/>
       <c r="J8" s="36" t="n"/>
-      <c r="K8" s="59" t="n"/>
+      <c r="K8" s="55" t="n"/>
       <c r="L8" s="36" t="n"/>
-      <c r="M8" s="59" t="n"/>
+      <c r="M8" s="55" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1" s="32">
-      <c r="A9" s="60" t="n">
+      <c r="A9" s="56" t="n">
         <v>45330</v>
       </c>
-      <c r="B9" s="33" t="n"/>
-      <c r="C9" s="57" t="n"/>
+      <c r="B9" s="60" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="C9" s="61" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="33" t="n"/>
-      <c r="E9" s="57" t="n"/>
+      <c r="E9" s="53" t="n"/>
       <c r="F9" s="33" t="n"/>
-      <c r="G9" s="57" t="n"/>
+      <c r="G9" s="53" t="n"/>
       <c r="H9" s="33" t="n"/>
-      <c r="I9" s="57" t="n"/>
+      <c r="I9" s="53" t="n"/>
       <c r="J9" s="33" t="n"/>
-      <c r="K9" s="57" t="n"/>
+      <c r="K9" s="53" t="n"/>
       <c r="L9" s="33" t="n"/>
-      <c r="M9" s="57" t="n"/>
+      <c r="M9" s="53" t="n"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="32">
-      <c r="A10" s="58" t="n">
+      <c r="A10" s="54" t="n">
         <v>45331</v>
       </c>
-      <c r="B10" s="36" t="n"/>
-      <c r="C10" s="59" t="n"/>
+      <c r="B10" s="62" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="C10" s="63" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D10" s="36" t="n"/>
-      <c r="E10" s="59" t="n"/>
+      <c r="E10" s="55" t="n"/>
       <c r="F10" s="36" t="n"/>
-      <c r="G10" s="59" t="n"/>
+      <c r="G10" s="55" t="n"/>
       <c r="H10" s="36" t="n"/>
-      <c r="I10" s="59" t="n"/>
+      <c r="I10" s="55" t="n"/>
       <c r="J10" s="36" t="n"/>
-      <c r="K10" s="59" t="n"/>
+      <c r="K10" s="55" t="n"/>
       <c r="L10" s="36" t="n"/>
-      <c r="M10" s="59" t="n"/>
+      <c r="M10" s="55" t="n"/>
     </row>
     <row r="11" ht="15" customHeight="1" s="32">
-      <c r="A11" s="61" t="n">
+      <c r="A11" s="57" t="n">
         <v>45332</v>
       </c>
-      <c r="B11" s="62" t="n"/>
-      <c r="C11" s="63" t="n"/>
-      <c r="D11" s="62" t="n"/>
-      <c r="E11" s="63" t="n"/>
-      <c r="F11" s="62" t="n"/>
-      <c r="G11" s="63" t="n"/>
-      <c r="H11" s="62" t="n"/>
-      <c r="I11" s="63" t="n"/>
-      <c r="J11" s="62" t="n"/>
-      <c r="K11" s="63" t="n"/>
-      <c r="L11" s="62" t="n"/>
-      <c r="M11" s="63" t="n"/>
+      <c r="B11" s="58" t="n"/>
+      <c r="C11" s="59" t="n"/>
+      <c r="D11" s="58" t="n"/>
+      <c r="E11" s="59" t="n"/>
+      <c r="F11" s="58" t="n"/>
+      <c r="G11" s="59" t="n"/>
+      <c r="H11" s="58" t="n"/>
+      <c r="I11" s="59" t="n"/>
+      <c r="J11" s="58" t="n"/>
+      <c r="K11" s="59" t="n"/>
+      <c r="L11" s="58" t="n"/>
+      <c r="M11" s="59" t="n"/>
     </row>
     <row r="12" ht="15" customHeight="1" s="32">
-      <c r="A12" s="61" t="n">
+      <c r="A12" s="57" t="n">
         <v>45333</v>
       </c>
-      <c r="B12" s="62" t="n"/>
-      <c r="C12" s="63" t="n"/>
-      <c r="D12" s="62" t="n"/>
-      <c r="E12" s="63" t="n"/>
-      <c r="F12" s="62" t="n"/>
-      <c r="G12" s="63" t="n"/>
-      <c r="H12" s="62" t="n"/>
-      <c r="I12" s="63" t="n"/>
-      <c r="J12" s="62" t="n"/>
-      <c r="K12" s="63" t="n"/>
-      <c r="L12" s="62" t="n"/>
-      <c r="M12" s="63" t="n"/>
+      <c r="B12" s="58" t="n"/>
+      <c r="C12" s="59" t="n"/>
+      <c r="D12" s="58" t="n"/>
+      <c r="E12" s="59" t="n"/>
+      <c r="F12" s="58" t="n"/>
+      <c r="G12" s="59" t="n"/>
+      <c r="H12" s="58" t="n"/>
+      <c r="I12" s="59" t="n"/>
+      <c r="J12" s="58" t="n"/>
+      <c r="K12" s="59" t="n"/>
+      <c r="L12" s="58" t="n"/>
+      <c r="M12" s="59" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1" s="32">
-      <c r="A13" s="60" t="n">
+      <c r="A13" s="56" t="n">
         <v>45334</v>
       </c>
-      <c r="B13" s="33" t="n"/>
-      <c r="C13" s="57" t="n"/>
+      <c r="B13" s="60" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="C13" s="61" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D13" s="33" t="n"/>
-      <c r="E13" s="57" t="n"/>
+      <c r="E13" s="53" t="n"/>
       <c r="F13" s="33" t="n"/>
-      <c r="G13" s="57" t="n"/>
+      <c r="G13" s="53" t="n"/>
       <c r="H13" s="33" t="n"/>
-      <c r="I13" s="57" t="n"/>
+      <c r="I13" s="53" t="n"/>
       <c r="J13" s="33" t="n"/>
-      <c r="K13" s="57" t="n"/>
+      <c r="K13" s="53" t="n"/>
       <c r="L13" s="33" t="n"/>
-      <c r="M13" s="57" t="n"/>
+      <c r="M13" s="53" t="n"/>
     </row>
     <row r="14" ht="15" customHeight="1" s="32">
-      <c r="A14" s="58" t="n">
+      <c r="A14" s="54" t="n">
         <v>45335</v>
       </c>
       <c r="B14" s="36" t="n"/>
-      <c r="C14" s="59" t="n"/>
+      <c r="C14" s="55" t="n"/>
       <c r="D14" s="36" t="n"/>
-      <c r="E14" s="59" t="n"/>
+      <c r="E14" s="55" t="n"/>
       <c r="F14" s="36" t="n"/>
-      <c r="G14" s="59" t="n"/>
+      <c r="G14" s="55" t="n"/>
       <c r="H14" s="36" t="n"/>
-      <c r="I14" s="59" t="n"/>
+      <c r="I14" s="55" t="n"/>
       <c r="J14" s="36" t="n"/>
-      <c r="K14" s="59" t="n"/>
+      <c r="K14" s="55" t="n"/>
       <c r="L14" s="36" t="n"/>
-      <c r="M14" s="59" t="n"/>
+      <c r="M14" s="55" t="n"/>
     </row>
     <row r="15" ht="15" customHeight="1" s="32">
-      <c r="A15" s="60" t="n">
+      <c r="A15" s="56" t="n">
         <v>45336</v>
       </c>
       <c r="B15" s="33" t="n"/>
-      <c r="C15" s="57" t="n"/>
+      <c r="C15" s="53" t="n"/>
       <c r="D15" s="33" t="n"/>
-      <c r="E15" s="57" t="n"/>
+      <c r="E15" s="53" t="n"/>
       <c r="F15" s="33" t="n"/>
-      <c r="G15" s="57" t="n"/>
+      <c r="G15" s="53" t="n"/>
       <c r="H15" s="33" t="n"/>
-      <c r="I15" s="57" t="n"/>
+      <c r="I15" s="53" t="n"/>
       <c r="J15" s="33" t="n"/>
-      <c r="K15" s="57" t="n"/>
+      <c r="K15" s="53" t="n"/>
       <c r="L15" s="33" t="n"/>
-      <c r="M15" s="57" t="n"/>
+      <c r="M15" s="53" t="n"/>
     </row>
     <row r="16" ht="15" customHeight="1" s="32">
-      <c r="A16" s="58" t="n">
+      <c r="A16" s="54" t="n">
         <v>45337</v>
       </c>
       <c r="B16" s="36" t="n"/>
-      <c r="C16" s="59" t="n"/>
+      <c r="C16" s="55" t="n"/>
       <c r="D16" s="36" t="n"/>
-      <c r="E16" s="59" t="n"/>
+      <c r="E16" s="55" t="n"/>
       <c r="F16" s="36" t="n"/>
-      <c r="G16" s="59" t="n"/>
+      <c r="G16" s="55" t="n"/>
       <c r="H16" s="36" t="n"/>
-      <c r="I16" s="59" t="n"/>
+      <c r="I16" s="55" t="n"/>
       <c r="J16" s="36" t="n"/>
-      <c r="K16" s="59" t="n"/>
+      <c r="K16" s="55" t="n"/>
       <c r="L16" s="36" t="n"/>
-      <c r="M16" s="59" t="n"/>
+      <c r="M16" s="55" t="n"/>
     </row>
     <row r="17" ht="15" customHeight="1" s="32">
-      <c r="A17" s="60" t="n">
+      <c r="A17" s="56" t="n">
         <v>45338</v>
       </c>
       <c r="B17" s="33" t="n"/>
-      <c r="C17" s="57" t="n"/>
+      <c r="C17" s="53" t="n"/>
       <c r="D17" s="33" t="n"/>
-      <c r="E17" s="57" t="n"/>
+      <c r="E17" s="53" t="n"/>
       <c r="F17" s="33" t="n"/>
-      <c r="G17" s="57" t="n"/>
+      <c r="G17" s="53" t="n"/>
       <c r="H17" s="33" t="n"/>
-      <c r="I17" s="57" t="n"/>
+      <c r="I17" s="53" t="n"/>
       <c r="J17" s="33" t="n"/>
-      <c r="K17" s="57" t="n"/>
+      <c r="K17" s="53" t="n"/>
       <c r="L17" s="33" t="n"/>
-      <c r="M17" s="57" t="n"/>
+      <c r="M17" s="53" t="n"/>
     </row>
     <row r="18" ht="15" customHeight="1" s="32">
-      <c r="A18" s="61" t="n">
+      <c r="A18" s="57" t="n">
         <v>45339</v>
       </c>
-      <c r="B18" s="62" t="n"/>
-      <c r="C18" s="63" t="n"/>
-      <c r="D18" s="62" t="n"/>
-      <c r="E18" s="63" t="n"/>
-      <c r="F18" s="62" t="n"/>
-      <c r="G18" s="63" t="n"/>
-      <c r="H18" s="62" t="n"/>
-      <c r="I18" s="63" t="n"/>
-      <c r="J18" s="62" t="n"/>
-      <c r="K18" s="63" t="n"/>
-      <c r="L18" s="62" t="n"/>
-      <c r="M18" s="63" t="n"/>
+      <c r="B18" s="58" t="n"/>
+      <c r="C18" s="59" t="n"/>
+      <c r="D18" s="58" t="n"/>
+      <c r="E18" s="59" t="n"/>
+      <c r="F18" s="58" t="n"/>
+      <c r="G18" s="59" t="n"/>
+      <c r="H18" s="58" t="n"/>
+      <c r="I18" s="59" t="n"/>
+      <c r="J18" s="58" t="n"/>
+      <c r="K18" s="59" t="n"/>
+      <c r="L18" s="58" t="n"/>
+      <c r="M18" s="59" t="n"/>
     </row>
     <row r="19" ht="15" customHeight="1" s="32">
-      <c r="A19" s="61" t="n">
+      <c r="A19" s="57" t="n">
         <v>45340</v>
       </c>
-      <c r="B19" s="62" t="n"/>
-      <c r="C19" s="63" t="n"/>
-      <c r="D19" s="62" t="n"/>
-      <c r="E19" s="63" t="n"/>
-      <c r="F19" s="62" t="n"/>
-      <c r="G19" s="63" t="n"/>
-      <c r="H19" s="62" t="n"/>
-      <c r="I19" s="63" t="n"/>
-      <c r="J19" s="62" t="n"/>
-      <c r="K19" s="63" t="n"/>
-      <c r="L19" s="62" t="n"/>
-      <c r="M19" s="63" t="n"/>
+      <c r="B19" s="58" t="n"/>
+      <c r="C19" s="59" t="n"/>
+      <c r="D19" s="58" t="n"/>
+      <c r="E19" s="59" t="n"/>
+      <c r="F19" s="58" t="n"/>
+      <c r="G19" s="59" t="n"/>
+      <c r="H19" s="58" t="n"/>
+      <c r="I19" s="59" t="n"/>
+      <c r="J19" s="58" t="n"/>
+      <c r="K19" s="59" t="n"/>
+      <c r="L19" s="58" t="n"/>
+      <c r="M19" s="59" t="n"/>
     </row>
     <row r="20" ht="15" customHeight="1" s="32">
-      <c r="A20" s="58" t="n">
+      <c r="A20" s="54" t="n">
         <v>45341</v>
       </c>
       <c r="B20" s="36" t="n"/>
-      <c r="C20" s="59" t="n"/>
+      <c r="C20" s="55" t="n"/>
       <c r="D20" s="36" t="n"/>
-      <c r="E20" s="59" t="n"/>
+      <c r="E20" s="55" t="n"/>
       <c r="F20" s="36" t="n"/>
-      <c r="G20" s="59" t="n"/>
+      <c r="G20" s="55" t="n"/>
       <c r="H20" s="36" t="n"/>
-      <c r="I20" s="59" t="n"/>
+      <c r="I20" s="55" t="n"/>
       <c r="J20" s="36" t="n"/>
-      <c r="K20" s="59" t="n"/>
+      <c r="K20" s="55" t="n"/>
       <c r="L20" s="36" t="n"/>
-      <c r="M20" s="59" t="n"/>
+      <c r="M20" s="55" t="n"/>
     </row>
     <row r="21" ht="15" customHeight="1" s="32">
-      <c r="A21" s="60" t="n">
+      <c r="A21" s="56" t="n">
         <v>45342</v>
       </c>
       <c r="B21" s="33" t="n"/>
-      <c r="C21" s="57" t="n"/>
+      <c r="C21" s="53" t="n"/>
       <c r="D21" s="33" t="n"/>
-      <c r="E21" s="57" t="n"/>
+      <c r="E21" s="53" t="n"/>
       <c r="F21" s="33" t="n"/>
-      <c r="G21" s="57" t="n"/>
+      <c r="G21" s="53" t="n"/>
       <c r="H21" s="33" t="n"/>
-      <c r="I21" s="57" t="n"/>
+      <c r="I21" s="53" t="n"/>
       <c r="J21" s="33" t="n"/>
-      <c r="K21" s="57" t="n"/>
+      <c r="K21" s="53" t="n"/>
       <c r="L21" s="33" t="n"/>
-      <c r="M21" s="57" t="n"/>
+      <c r="M21" s="53" t="n"/>
     </row>
     <row r="22" ht="15" customHeight="1" s="32">
-      <c r="A22" s="58" t="n">
+      <c r="A22" s="54" t="n">
         <v>45343</v>
       </c>
       <c r="B22" s="36" t="n"/>
-      <c r="C22" s="59" t="n"/>
+      <c r="C22" s="55" t="n"/>
       <c r="D22" s="36" t="n"/>
-      <c r="E22" s="59" t="n"/>
+      <c r="E22" s="55" t="n"/>
       <c r="F22" s="36" t="n"/>
-      <c r="G22" s="59" t="n"/>
+      <c r="G22" s="55" t="n"/>
       <c r="H22" s="36" t="n"/>
-      <c r="I22" s="59" t="n"/>
+      <c r="I22" s="55" t="n"/>
       <c r="J22" s="36" t="n"/>
-      <c r="K22" s="59" t="n"/>
+      <c r="K22" s="55" t="n"/>
       <c r="L22" s="36" t="n"/>
-      <c r="M22" s="59" t="n"/>
+      <c r="M22" s="55" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" s="32">
-      <c r="A23" s="60" t="n">
+      <c r="A23" s="56" t="n">
         <v>45344</v>
       </c>
       <c r="B23" s="33" t="n"/>
-      <c r="C23" s="57" t="n"/>
+      <c r="C23" s="53" t="n"/>
       <c r="D23" s="33" t="n"/>
-      <c r="E23" s="57" t="n"/>
+      <c r="E23" s="53" t="n"/>
       <c r="F23" s="33" t="n"/>
-      <c r="G23" s="57" t="n"/>
+      <c r="G23" s="53" t="n"/>
       <c r="H23" s="33" t="n"/>
-      <c r="I23" s="57" t="n"/>
+      <c r="I23" s="53" t="n"/>
       <c r="J23" s="33" t="n"/>
-      <c r="K23" s="57" t="n"/>
+      <c r="K23" s="53" t="n"/>
       <c r="L23" s="33" t="n"/>
-      <c r="M23" s="57" t="n"/>
+      <c r="M23" s="53" t="n"/>
     </row>
     <row r="24" ht="15" customHeight="1" s="32">
-      <c r="A24" s="58" t="n">
+      <c r="A24" s="54" t="n">
         <v>45345</v>
       </c>
       <c r="B24" s="36" t="n"/>
-      <c r="C24" s="59" t="n"/>
+      <c r="C24" s="55" t="n"/>
       <c r="D24" s="36" t="n"/>
-      <c r="E24" s="59" t="n"/>
+      <c r="E24" s="55" t="n"/>
       <c r="F24" s="36" t="n"/>
-      <c r="G24" s="59" t="n"/>
+      <c r="G24" s="55" t="n"/>
       <c r="H24" s="36" t="n"/>
-      <c r="I24" s="59" t="n"/>
+      <c r="I24" s="55" t="n"/>
       <c r="J24" s="36" t="n"/>
-      <c r="K24" s="59" t="n"/>
+      <c r="K24" s="55" t="n"/>
       <c r="L24" s="36" t="n"/>
-      <c r="M24" s="59" t="n"/>
+      <c r="M24" s="55" t="n"/>
     </row>
     <row r="25" ht="15" customHeight="1" s="32">
-      <c r="A25" s="61" t="n">
+      <c r="A25" s="57" t="n">
         <v>45346</v>
       </c>
-      <c r="B25" s="62" t="n"/>
-      <c r="C25" s="63" t="n"/>
-      <c r="D25" s="62" t="n"/>
-      <c r="E25" s="63" t="n"/>
-      <c r="F25" s="62" t="n"/>
-      <c r="G25" s="63" t="n"/>
-      <c r="H25" s="62" t="n"/>
-      <c r="I25" s="63" t="n"/>
-      <c r="J25" s="62" t="n"/>
-      <c r="K25" s="63" t="n"/>
-      <c r="L25" s="62" t="n"/>
-      <c r="M25" s="63" t="n"/>
+      <c r="B25" s="58" t="n"/>
+      <c r="C25" s="59" t="n"/>
+      <c r="D25" s="58" t="n"/>
+      <c r="E25" s="59" t="n"/>
+      <c r="F25" s="58" t="n"/>
+      <c r="G25" s="59" t="n"/>
+      <c r="H25" s="58" t="n"/>
+      <c r="I25" s="59" t="n"/>
+      <c r="J25" s="58" t="n"/>
+      <c r="K25" s="59" t="n"/>
+      <c r="L25" s="58" t="n"/>
+      <c r="M25" s="59" t="n"/>
     </row>
     <row r="26" ht="15" customHeight="1" s="32">
-      <c r="A26" s="61" t="n">
+      <c r="A26" s="57" t="n">
         <v>45347</v>
       </c>
-      <c r="B26" s="62" t="n"/>
-      <c r="C26" s="63" t="n"/>
-      <c r="D26" s="62" t="n"/>
-      <c r="E26" s="63" t="n"/>
-      <c r="F26" s="62" t="n"/>
-      <c r="G26" s="63" t="n"/>
-      <c r="H26" s="62" t="n"/>
-      <c r="I26" s="63" t="n"/>
-      <c r="J26" s="62" t="n"/>
-      <c r="K26" s="63" t="n"/>
-      <c r="L26" s="62" t="n"/>
-      <c r="M26" s="63" t="n"/>
+      <c r="B26" s="58" t="n"/>
+      <c r="C26" s="59" t="n"/>
+      <c r="D26" s="58" t="n"/>
+      <c r="E26" s="59" t="n"/>
+      <c r="F26" s="58" t="n"/>
+      <c r="G26" s="59" t="n"/>
+      <c r="H26" s="58" t="n"/>
+      <c r="I26" s="59" t="n"/>
+      <c r="J26" s="58" t="n"/>
+      <c r="K26" s="59" t="n"/>
+      <c r="L26" s="58" t="n"/>
+      <c r="M26" s="59" t="n"/>
     </row>
     <row r="27" ht="15" customHeight="1" s="32">
-      <c r="A27" s="60" t="n">
+      <c r="A27" s="56" t="n">
         <v>45348</v>
       </c>
       <c r="B27" s="33" t="n"/>
-      <c r="C27" s="57" t="n"/>
+      <c r="C27" s="53" t="n"/>
       <c r="D27" s="33" t="n"/>
-      <c r="E27" s="57" t="n"/>
+      <c r="E27" s="53" t="n"/>
       <c r="F27" s="33" t="n"/>
-      <c r="G27" s="57" t="n"/>
+      <c r="G27" s="53" t="n"/>
       <c r="H27" s="33" t="n"/>
-      <c r="I27" s="57" t="n"/>
+      <c r="I27" s="53" t="n"/>
       <c r="J27" s="33" t="n"/>
-      <c r="K27" s="57" t="n"/>
+      <c r="K27" s="53" t="n"/>
       <c r="L27" s="33" t="n"/>
-      <c r="M27" s="57" t="n"/>
+      <c r="M27" s="53" t="n"/>
     </row>
     <row r="28" ht="15" customHeight="1" s="32">
-      <c r="A28" s="58" t="n">
+      <c r="A28" s="54" t="n">
         <v>45349</v>
       </c>
       <c r="B28" s="36" t="n"/>
-      <c r="C28" s="59" t="n"/>
+      <c r="C28" s="55" t="n"/>
       <c r="D28" s="36" t="n"/>
-      <c r="E28" s="59" t="n"/>
+      <c r="E28" s="55" t="n"/>
       <c r="F28" s="36" t="n"/>
-      <c r="G28" s="59" t="n"/>
+      <c r="G28" s="55" t="n"/>
       <c r="H28" s="36" t="n"/>
-      <c r="I28" s="59" t="n"/>
+      <c r="I28" s="55" t="n"/>
       <c r="J28" s="36" t="n"/>
-      <c r="K28" s="59" t="n"/>
+      <c r="K28" s="55" t="n"/>
       <c r="L28" s="36" t="n"/>
-      <c r="M28" s="59" t="n"/>
+      <c r="M28" s="55" t="n"/>
     </row>
     <row r="29" ht="15" customHeight="1" s="32">
-      <c r="A29" s="60" t="n">
+      <c r="A29" s="56" t="n">
         <v>45350</v>
       </c>
       <c r="B29" s="33" t="n"/>
-      <c r="C29" s="57" t="n"/>
+      <c r="C29" s="53" t="n"/>
       <c r="D29" s="33" t="n"/>
-      <c r="E29" s="57" t="n"/>
+      <c r="E29" s="53" t="n"/>
       <c r="F29" s="33" t="n"/>
-      <c r="G29" s="57" t="n"/>
+      <c r="G29" s="53" t="n"/>
       <c r="H29" s="33" t="n"/>
-      <c r="I29" s="57" t="n"/>
+      <c r="I29" s="53" t="n"/>
       <c r="J29" s="33" t="n"/>
-      <c r="K29" s="57" t="n"/>
+      <c r="K29" s="53" t="n"/>
       <c r="L29" s="33" t="n"/>
-      <c r="M29" s="57" t="n"/>
+      <c r="M29" s="53" t="n"/>
     </row>
     <row r="30" ht="15" customHeight="1" s="32">
-      <c r="A30" s="58" t="n">
+      <c r="A30" s="54" t="n">
         <v>45351</v>
       </c>
       <c r="B30" s="36" t="n"/>
-      <c r="C30" s="59" t="n"/>
+      <c r="C30" s="55" t="n"/>
       <c r="D30" s="36" t="n"/>
-      <c r="E30" s="59" t="n"/>
+      <c r="E30" s="55" t="n"/>
       <c r="F30" s="36" t="n"/>
-      <c r="G30" s="59" t="n"/>
+      <c r="G30" s="55" t="n"/>
       <c r="H30" s="36" t="n"/>
-      <c r="I30" s="59" t="n"/>
+      <c r="I30" s="55" t="n"/>
       <c r="J30" s="36" t="n"/>
-      <c r="K30" s="59" t="n"/>
+      <c r="K30" s="55" t="n"/>
       <c r="L30" s="36" t="n"/>
-      <c r="M30" s="59" t="n"/>
+      <c r="M30" s="55" t="n"/>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="32"/>
     <row r="32" ht="13.5" customHeight="1" s="32"/>

</xml_diff>